<commit_message>
Refreshing work to current
</commit_message>
<xml_diff>
--- a/EmployeeSQL/m9-starter-code/Starter_Code/data/Snapshot_of_Tables.xlsx
+++ b/EmployeeSQL/m9-starter-code/Starter_Code/data/Snapshot_of_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grigor\Desktop\Weekly  Classes\challenges\sql-challenge\EmployeeSQL\m9-starter-code\Starter_Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C027CD88-E510-42D9-B2B8-B97ABBCFE7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCA9BFF-D65C-4491-B8BD-978793C54C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38145" yWindow="870" windowWidth="16515" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>Departments</t>
   </si>
@@ -341,6 +341,29 @@
         <scheme val="minor"/>
       </rPr>
       <t>department_id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> employees_id</t>
     </r>
   </si>
 </sst>
@@ -726,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1070,7 @@
         <v>36</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>